<commit_message>
Predictions by year and species
Modifications to adapt predictions by year and predictions by species to revision requirements
</commit_message>
<xml_diff>
--- a/results/ALLFEATURES_100.xlsx
+++ b/results/ALLFEATURES_100.xlsx
@@ -375,1102 +375,1102 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>1270.630445882262</v>
+        <v>1407.210685131796</v>
       </c>
       <c r="B2">
-        <v>35.64590363396981</v>
+        <v>37.51280694818499</v>
       </c>
       <c r="C2">
-        <v>0.9270360735167512</v>
+        <v>0.9044773135778155</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>1268.347371221075</v>
+        <v>1406.702963604032</v>
       </c>
       <c r="B3">
-        <v>35.61386487340394</v>
+        <v>37.50603902845556</v>
       </c>
       <c r="C3">
-        <v>0.914254498327557</v>
+        <v>0.9041509782192719</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>1405.488262802591</v>
+        <v>1407.742326933311</v>
       </c>
       <c r="B4">
-        <v>37.48984212826978</v>
+        <v>37.51989241633444</v>
       </c>
       <c r="C4">
-        <v>0.8913298024455402</v>
+        <v>0.9048190235672956</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>1427.008356901882</v>
+        <v>1409.998896583282</v>
       </c>
       <c r="B5">
-        <v>37.77576414716031</v>
+        <v>37.54995201838855</v>
       </c>
       <c r="C5">
-        <v>0.9023026043465879</v>
+        <v>0.9062694219166529</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>1497.031460138884</v>
+        <v>1407.778220819908</v>
       </c>
       <c r="B6">
-        <v>38.69149079757569</v>
+        <v>37.52037074470225</v>
       </c>
       <c r="C6">
-        <v>0.8919678521059965</v>
+        <v>0.9048420941753298</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>1289.906163753173</v>
+        <v>1406.230420578581</v>
       </c>
       <c r="B7">
-        <v>35.9152636598031</v>
+        <v>37.49973894013905</v>
       </c>
       <c r="C7">
-        <v>0.9102536523230285</v>
+        <v>0.9038472536592453</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>1469.364577605104</v>
+        <v>1404.735221757981</v>
       </c>
       <c r="B8">
-        <v>38.33229157779514</v>
+        <v>37.47979751490102</v>
       </c>
       <c r="C8">
-        <v>0.8931302793543447</v>
+        <v>0.9028862224314308</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>1417.170671573495</v>
+        <v>1407.818883415257</v>
       </c>
       <c r="B9">
-        <v>37.64532735378317</v>
+        <v>37.52091261437089</v>
       </c>
       <c r="C9">
-        <v>0.9038269328156981</v>
+        <v>0.9048682298459824</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>1444.839936952436</v>
+        <v>1408.279102286829</v>
       </c>
       <c r="B10">
-        <v>38.01105019533709</v>
+        <v>37.52704494477056</v>
       </c>
       <c r="C10">
-        <v>0.8852712047873724</v>
+        <v>0.9051640331205</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>1231.544374268112</v>
+        <v>1408.633716157295</v>
       </c>
       <c r="B11">
-        <v>35.09336652799375</v>
+        <v>37.53176942481256</v>
       </c>
       <c r="C11">
-        <v>0.9319295062270713</v>
+        <v>0.9053919593324971</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>1330.88781985888</v>
+        <v>1406.54721640977</v>
       </c>
       <c r="B12">
-        <v>36.48133522582309</v>
+        <v>37.50396267609291</v>
       </c>
       <c r="C12">
-        <v>0.9169017768696383</v>
+        <v>0.9040508725241191</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>1502.342141726547</v>
+        <v>1407.864329340877</v>
       </c>
       <c r="B13">
-        <v>38.76005858775947</v>
+        <v>37.52151821742928</v>
       </c>
       <c r="C13">
-        <v>0.889799528182025</v>
+        <v>0.9048974399771587</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>1416.107966183992</v>
+        <v>1408.879737310668</v>
       </c>
       <c r="B14">
-        <v>37.63121000159298</v>
+        <v>37.53504678711175</v>
       </c>
       <c r="C14">
-        <v>0.8983705098285947</v>
+        <v>0.9055500881430709</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>1305.895032190458</v>
+        <v>1405.358583877117</v>
       </c>
       <c r="B15">
-        <v>36.13716967597847</v>
+        <v>37.48811256754756</v>
       </c>
       <c r="C15">
-        <v>0.9081111035763253</v>
+        <v>0.9032868851757224</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>1216.83234566132</v>
+        <v>1407.500022073736</v>
       </c>
       <c r="B16">
-        <v>34.88312408115591</v>
+        <v>37.5166632587939</v>
       </c>
       <c r="C16">
-        <v>0.914952647987231</v>
+        <v>0.9046632833851379</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>1476.439733908519</v>
+        <v>1408.389482518538</v>
       </c>
       <c r="B17">
-        <v>38.42446790664145</v>
+        <v>37.52851559172755</v>
       </c>
       <c r="C17">
-        <v>0.8992054490577838</v>
+        <v>0.9052349794375814</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>1429.733844738532</v>
+        <v>1404.170806872062</v>
       </c>
       <c r="B18">
-        <v>37.81182149458727</v>
+        <v>37.47226717016282</v>
       </c>
       <c r="C18">
-        <v>0.9040507956025282</v>
+        <v>0.9025234477132134</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>1390.708003984409</v>
+        <v>1411.497514862248</v>
       </c>
       <c r="B19">
-        <v>37.29219762878569</v>
+        <v>37.56990171483348</v>
       </c>
       <c r="C19">
-        <v>0.904809425953048</v>
+        <v>0.9072326509834556</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>1449.38534239093</v>
+        <v>1405.773215591014</v>
       </c>
       <c r="B20">
-        <v>38.07079382401857</v>
+        <v>37.49364233561489</v>
       </c>
       <c r="C20">
-        <v>0.903304548812951</v>
+        <v>0.9035533875429025</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>1390.39173556327</v>
+        <v>1405.56655454796</v>
       </c>
       <c r="B21">
-        <v>37.28795697759894</v>
+        <v>37.49088628650915</v>
       </c>
       <c r="C21">
-        <v>0.8995745071944924</v>
+        <v>0.9034205572375248</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>1493.531197771116</v>
+        <v>1411.621299467631</v>
       </c>
       <c r="B22">
-        <v>38.64623135276085</v>
+        <v>37.57154906931082</v>
       </c>
       <c r="C22">
-        <v>0.8885978728438562</v>
+        <v>0.9073122128916534</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>1325.663005652863</v>
+        <v>1405.785630204893</v>
       </c>
       <c r="B23">
-        <v>36.40965539047112</v>
+        <v>37.49380789150247</v>
       </c>
       <c r="C23">
-        <v>0.9078237823203259</v>
+        <v>0.9035613669710941</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>1387.046773329231</v>
+        <v>1407.675675259082</v>
       </c>
       <c r="B24">
-        <v>37.24307685099649</v>
+        <v>37.51900418799894</v>
       </c>
       <c r="C24">
-        <v>0.8842331342892411</v>
+        <v>0.9047761835520263</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>1346.723572425986</v>
+        <v>1406.457023527306</v>
       </c>
       <c r="B25">
-        <v>36.69773252431253</v>
+        <v>37.5027602121138</v>
       </c>
       <c r="C25">
-        <v>0.8982186355650958</v>
+        <v>0.9039929015202666</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>1359.083127295673</v>
+        <v>1405.378671144655</v>
       </c>
       <c r="B26">
-        <v>36.86574463232328</v>
+        <v>37.48838048175267</v>
       </c>
       <c r="C26">
-        <v>0.900336427990727</v>
+        <v>0.9032997961619581</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>1380.272497078434</v>
+        <v>1408.002750090022</v>
       </c>
       <c r="B27">
-        <v>37.15201874835921</v>
+        <v>37.52336272364221</v>
       </c>
       <c r="C27">
-        <v>0.8985918170382389</v>
+        <v>0.9049864091902636</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>1402.94981862846</v>
+        <v>1405.428354552094</v>
       </c>
       <c r="B28">
-        <v>37.45597173520478</v>
+        <v>37.48904312665361</v>
       </c>
       <c r="C28">
-        <v>0.9084236464908227</v>
+        <v>0.9033317299124392</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>1464.490272203373</v>
+        <v>1407.488449859894</v>
       </c>
       <c r="B29">
-        <v>38.26865913777714</v>
+        <v>37.51650903082394</v>
       </c>
       <c r="C29">
-        <v>0.8899484353152856</v>
+        <v>0.9046558454051511</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>1393.20105220607</v>
+        <v>1403.347988726328</v>
       </c>
       <c r="B30">
-        <v>37.32560853095458</v>
+        <v>37.46128653325093</v>
       </c>
       <c r="C30">
-        <v>0.9059816847450305</v>
+        <v>0.9019945856502289</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>1510.91257341912</v>
+        <v>1405.557398866767</v>
       </c>
       <c r="B31">
-        <v>38.87045887842232</v>
+        <v>37.4907641808855</v>
       </c>
       <c r="C31">
-        <v>0.8881397164447976</v>
+        <v>0.9034146724712805</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>1326.530716172201</v>
+        <v>1406.433180674311</v>
       </c>
       <c r="B32">
-        <v>36.42156938096163</v>
+        <v>37.50244232945784</v>
       </c>
       <c r="C32">
-        <v>0.9134477020487439</v>
+        <v>0.9039775766511199</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>1438.050833506557</v>
+        <v>1408.840265668796</v>
       </c>
       <c r="B33">
-        <v>37.92164070167003</v>
+        <v>37.53452098627071</v>
       </c>
       <c r="C33">
-        <v>0.8959898404085589</v>
+        <v>0.9055247179515388</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>1419.529057804552</v>
+        <v>1408.147209760708</v>
       </c>
       <c r="B34">
-        <v>37.67663809052703</v>
+        <v>37.52528760397058</v>
       </c>
       <c r="C34">
-        <v>0.8932159950476914</v>
+        <v>0.9050792598886348</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>1453.219103473433</v>
+        <v>1407.782915805828</v>
       </c>
       <c r="B35">
-        <v>38.12111099474191</v>
+        <v>37.52043331047535</v>
       </c>
       <c r="C35">
-        <v>0.8975752920239938</v>
+        <v>0.9048451118529874</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>1224.101733259356</v>
+        <v>1405.453096207635</v>
       </c>
       <c r="B36">
-        <v>34.98716526469894</v>
+        <v>37.48937311035802</v>
       </c>
       <c r="C36">
-        <v>0.9255593378873277</v>
+        <v>0.903347632482227</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>1395.058486996105</v>
+        <v>1404.17274869948</v>
       </c>
       <c r="B37">
-        <v>37.35048175052238</v>
+        <v>37.47229308034778</v>
       </c>
       <c r="C37">
-        <v>0.9004317128034716</v>
+        <v>0.9025246958126464</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>1294.948168264979</v>
+        <v>1408.21744756995</v>
       </c>
       <c r="B38">
-        <v>35.98538826058402</v>
+        <v>37.52622346533087</v>
       </c>
       <c r="C38">
-        <v>0.9104370421931292</v>
+        <v>0.9051244048734444</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>1360.054962223996</v>
+        <v>1404.986960261976</v>
       </c>
       <c r="B39">
-        <v>36.87892300791871</v>
+        <v>37.48315568708131</v>
       </c>
       <c r="C39">
-        <v>0.8952449867256147</v>
+        <v>0.9030480260392468</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>1331.61119730493</v>
+        <v>1407.988410040422</v>
       </c>
       <c r="B40">
-        <v>36.49124822892374</v>
+        <v>37.52317164153934</v>
       </c>
       <c r="C40">
-        <v>0.8884870865461946</v>
+        <v>0.9049771921983231</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>1421.455823118986</v>
+        <v>1405.879310860384</v>
       </c>
       <c r="B41">
-        <v>37.70219918146667</v>
+        <v>37.49505715238189</v>
       </c>
       <c r="C41">
-        <v>0.8853810852591207</v>
+        <v>0.9036215797228214</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
-        <v>1454.53024122792</v>
+        <v>1404.340559728315</v>
       </c>
       <c r="B42">
-        <v>38.13830412102667</v>
+        <v>37.47453214822455</v>
       </c>
       <c r="C42">
-        <v>0.8917456449180924</v>
+        <v>0.9026325554744327</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43">
-        <v>1438.021051416338</v>
+        <v>1406.338996627751</v>
       </c>
       <c r="B43">
-        <v>37.92124802028986</v>
+        <v>37.50118660292966</v>
       </c>
       <c r="C43">
-        <v>0.8926231781291564</v>
+        <v>0.9039170403474108</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44">
-        <v>1383.141453810161</v>
+        <v>1405.371702631222</v>
       </c>
       <c r="B44">
-        <v>37.19060975313744</v>
+        <v>37.48828753932649</v>
       </c>
       <c r="C44">
-        <v>0.8970795920703821</v>
+        <v>0.90329531718637</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45">
-        <v>1500.388012905494</v>
+        <v>1407.225029516207</v>
       </c>
       <c r="B45">
-        <v>38.7348423632457</v>
+        <v>37.51299814086055</v>
       </c>
       <c r="C45">
-        <v>0.8851184033987917</v>
+        <v>0.9044865333559308</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46">
-        <v>1348.317362212932</v>
+        <v>1407.182067205959</v>
       </c>
       <c r="B46">
-        <v>36.71944120235126</v>
+        <v>37.51242550417074</v>
       </c>
       <c r="C46">
-        <v>0.9018127472262526</v>
+        <v>0.9044589195555417</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>1508.545667769773</v>
+        <v>1406.499907975159</v>
       </c>
       <c r="B47">
-        <v>38.84000087242241</v>
+        <v>37.5033319583095</v>
       </c>
       <c r="C47">
-        <v>0.8922544816836828</v>
+        <v>0.9040204652750073</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>1326.80070757032</v>
+        <v>1405.784909488379</v>
       </c>
       <c r="B48">
-        <v>36.42527566910537</v>
+        <v>37.49379828036071</v>
       </c>
       <c r="C48">
-        <v>0.8999184024178303</v>
+        <v>0.9035609037343221</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49">
-        <v>1310.717048499267</v>
+        <v>1410.810010145072</v>
       </c>
       <c r="B49">
-        <v>36.20382643449815</v>
+        <v>37.56075092626705</v>
       </c>
       <c r="C49">
-        <v>0.9029837236705178</v>
+        <v>0.906790760919497</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50">
-        <v>1380.650050141574</v>
+        <v>1405.071145239746</v>
       </c>
       <c r="B50">
-        <v>37.1570995926966</v>
+        <v>37.48427864104824</v>
       </c>
       <c r="C50">
-        <v>0.8917697576488317</v>
+        <v>0.9031021354937513</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51">
-        <v>1408.559505368894</v>
+        <v>1407.343670968068</v>
       </c>
       <c r="B51">
-        <v>37.53078077217278</v>
+        <v>37.51457944543785</v>
       </c>
       <c r="C51">
-        <v>0.9008689050324016</v>
+        <v>0.9045627895290747</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52">
-        <v>1379.8599205766</v>
+        <v>1408.075313344974</v>
       </c>
       <c r="B52">
-        <v>37.14646578850537</v>
+        <v>37.5243296188616</v>
       </c>
       <c r="C52">
-        <v>0.8969292654072566</v>
+        <v>0.9050330488431632</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53">
-        <v>1450.850987111282</v>
+        <v>1406.070288952747</v>
       </c>
       <c r="B53">
-        <v>38.09003789852777</v>
+        <v>37.49760377614478</v>
       </c>
       <c r="C53">
-        <v>0.8936436788775471</v>
+        <v>0.9037443298936195</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54">
-        <v>1347.93871404425</v>
+        <v>1406.299560720708</v>
       </c>
       <c r="B54">
-        <v>36.71428487720072</v>
+        <v>37.50066080378728</v>
       </c>
       <c r="C54">
-        <v>0.909579774141929</v>
+        <v>0.903891693124258</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55">
-        <v>1419.381653576607</v>
+        <v>1409.821623043287</v>
       </c>
       <c r="B55">
-        <v>37.67468186430519</v>
+        <v>37.54759144130668</v>
       </c>
       <c r="C55">
-        <v>0.8927653919777361</v>
+        <v>0.9061554802752726</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56">
-        <v>1548.720466916792</v>
+        <v>1405.583876594934</v>
       </c>
       <c r="B56">
-        <v>39.35378592863452</v>
+        <v>37.49111730256828</v>
       </c>
       <c r="C56">
-        <v>0.8863463414874221</v>
+        <v>0.9034316908926849</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57">
-        <v>1447.586439106028</v>
+        <v>1407.159860947487</v>
       </c>
       <c r="B57">
-        <v>38.04716072331848</v>
+        <v>37.51212951763052</v>
       </c>
       <c r="C57">
-        <v>0.9049060043677328</v>
+        <v>0.904444646598966</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58">
-        <v>1388.72656672781</v>
+        <v>1407.211570724831</v>
       </c>
       <c r="B58">
-        <v>37.26562178104385</v>
+        <v>37.51281875205902</v>
       </c>
       <c r="C58">
-        <v>0.9073540454868781</v>
+        <v>0.9044778827881115</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59">
-        <v>1529.542026161852</v>
+        <v>1405.107917667765</v>
       </c>
       <c r="B59">
-        <v>39.10935982807507</v>
+        <v>37.4847691425166</v>
       </c>
       <c r="C59">
-        <v>0.9050919900355429</v>
+        <v>0.9031257707796796</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60">
-        <v>1330.996605452123</v>
+        <v>1407.291312002816</v>
       </c>
       <c r="B60">
-        <v>36.48282617139362</v>
+        <v>37.51388159072339</v>
       </c>
       <c r="C60">
-        <v>0.9135364183319556</v>
+        <v>0.904529136077792</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61">
-        <v>1338.036086478007</v>
+        <v>1406.757431416264</v>
       </c>
       <c r="B61">
-        <v>36.57917558499653</v>
+        <v>37.50676514198823</v>
       </c>
       <c r="C61">
-        <v>0.901065163441188</v>
+        <v>0.9041859871209289</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62">
-        <v>1533.822845390239</v>
+        <v>1406.089490509984</v>
       </c>
       <c r="B62">
-        <v>39.1640504211482</v>
+        <v>37.49785981239441</v>
       </c>
       <c r="C62">
-        <v>0.8894523344218578</v>
+        <v>0.9037566715941641</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63">
-        <v>1486.787568378461</v>
+        <v>1406.081501819863</v>
       </c>
       <c r="B63">
-        <v>38.55888442860427</v>
+        <v>37.49775329029544</v>
       </c>
       <c r="C63">
-        <v>0.8824743285648413</v>
+        <v>0.9037515369053432</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64">
-        <v>1656.493919553597</v>
+        <v>1407.391310889644</v>
       </c>
       <c r="B64">
-        <v>40.70004815173561</v>
+        <v>37.51521439215887</v>
       </c>
       <c r="C64">
-        <v>0.8922661369748157</v>
+        <v>0.9045934098396973</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65">
-        <v>1561.252414368573</v>
+        <v>1406.93670411301</v>
       </c>
       <c r="B65">
-        <v>39.51268675208728</v>
+        <v>37.5091549373351</v>
       </c>
       <c r="C65">
-        <v>0.8754898387252533</v>
+        <v>0.9043012137098579</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66">
-        <v>1417.722442592259</v>
+        <v>1407.102963774715</v>
       </c>
       <c r="B66">
-        <v>37.65265518648398</v>
+        <v>37.51137112629603</v>
       </c>
       <c r="C66">
-        <v>0.8906193340793698</v>
+        <v>0.9044080762385207</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67">
-        <v>1316.892208242266</v>
+        <v>1407.498283115443</v>
       </c>
       <c r="B67">
-        <v>36.28900946901508</v>
+        <v>37.51664008297442</v>
       </c>
       <c r="C67">
-        <v>0.9006594287748552</v>
+        <v>0.904662165678769</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68">
-        <v>1238.665690415724</v>
+        <v>1406.35246626413</v>
       </c>
       <c r="B68">
-        <v>35.19468270088146</v>
+        <v>37.50136619196866</v>
       </c>
       <c r="C68">
-        <v>0.928184658118819</v>
+        <v>0.903925697885801</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69">
-        <v>1392.626594771039</v>
+        <v>1405.65490424841</v>
       </c>
       <c r="B69">
-        <v>37.31791251893705</v>
+        <v>37.49206455036065</v>
       </c>
       <c r="C69">
-        <v>0.902156686199998</v>
+        <v>0.9034773435457634</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70">
-        <v>1515.91047268653</v>
+        <v>1405.93683849725</v>
       </c>
       <c r="B70">
-        <v>38.93469497359046</v>
+        <v>37.49582428080826</v>
       </c>
       <c r="C70">
-        <v>0.8775046705923446</v>
+        <v>0.9036585553107722</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71">
-        <v>1388.918536590337</v>
+        <v>1406.373827037288</v>
       </c>
       <c r="B71">
-        <v>37.26819738852869</v>
+        <v>37.50165099082023</v>
       </c>
       <c r="C71">
-        <v>0.9033761872649275</v>
+        <v>0.9039394274111141</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72">
-        <v>1461.141140317688</v>
+        <v>1405.714649715266</v>
       </c>
       <c r="B72">
-        <v>38.22487593593586</v>
+        <v>37.49286131672623</v>
       </c>
       <c r="C72">
-        <v>0.9021819357962944</v>
+        <v>0.9035157446323405</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73">
-        <v>1603.133157470796</v>
+        <v>1404.305384757741</v>
       </c>
       <c r="B73">
-        <v>40.03914531393991</v>
+        <v>37.47406282694393</v>
       </c>
       <c r="C73">
-        <v>0.8903949517740967</v>
+        <v>0.9026099469459086</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74">
-        <v>1379.733917754745</v>
+        <v>1406.40661641201</v>
       </c>
       <c r="B74">
-        <v>37.14476972273142</v>
+        <v>37.50208816068793</v>
       </c>
       <c r="C74">
-        <v>0.8987232203683283</v>
+        <v>0.903960502610353</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75">
-        <v>1522.179056484177</v>
+        <v>1404.810949339623</v>
       </c>
       <c r="B75">
-        <v>39.01511318046094</v>
+        <v>37.48080774662711</v>
       </c>
       <c r="C75">
-        <v>0.8955392460043013</v>
+        <v>0.9029348959387665</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76">
-        <v>1349.069713636755</v>
+        <v>1406.908387798265</v>
       </c>
       <c r="B76">
-        <v>36.72968436614661</v>
+        <v>37.50877747672224</v>
       </c>
       <c r="C76">
-        <v>0.8951910083302367</v>
+        <v>0.9042830135465412</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77">
-        <v>1472.304983679687</v>
+        <v>1404.572739944901</v>
       </c>
       <c r="B77">
-        <v>38.37062657397827</v>
+        <v>37.47762986029</v>
       </c>
       <c r="C77">
-        <v>0.8792734632364323</v>
+        <v>0.9027817880952266</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78">
-        <v>1424.173361291971</v>
+        <v>1407.047194634295</v>
       </c>
       <c r="B78">
-        <v>37.73822149084362</v>
+        <v>37.51062775580135</v>
       </c>
       <c r="C78">
-        <v>0.8886213940243264</v>
+        <v>0.9043722309149679</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79">
-        <v>1533.928766303297</v>
+        <v>1411.135155920036</v>
       </c>
       <c r="B79">
-        <v>39.16540267000069</v>
+        <v>37.56507894201789</v>
       </c>
       <c r="C79">
-        <v>0.8907740447850045</v>
+        <v>0.9069997466670889</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80">
-        <v>1397.440454754832</v>
+        <v>1407.390804482558</v>
       </c>
       <c r="B80">
-        <v>37.38235485833967</v>
+        <v>37.51520764280212</v>
       </c>
       <c r="C80">
-        <v>0.9043091553698902</v>
+        <v>0.9045930843491821</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81">
-        <v>1474.44343088925</v>
+        <v>1406.208211848012</v>
       </c>
       <c r="B81">
-        <v>38.39848214303854</v>
+        <v>37.49944282050083</v>
       </c>
       <c r="C81">
-        <v>0.8880852930843655</v>
+        <v>0.9038329791137375</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82">
-        <v>1512.091371462742</v>
+        <v>1408.093345860285</v>
       </c>
       <c r="B82">
-        <v>38.88561908293016</v>
+        <v>37.52456989574011</v>
       </c>
       <c r="C82">
-        <v>0.8939250455862318</v>
+        <v>0.9050446391481362</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83">
-        <v>1414.77682675379</v>
+        <v>1406.077081584038</v>
       </c>
       <c r="B83">
-        <v>37.61351920192778</v>
+        <v>37.49769435024023</v>
       </c>
       <c r="C83">
-        <v>0.8975763264209513</v>
+        <v>0.9037486958218752</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84">
-        <v>1356.034773875153</v>
+        <v>1405.683724573247</v>
       </c>
       <c r="B84">
-        <v>36.82437744042869</v>
+        <v>37.49244890072195</v>
       </c>
       <c r="C84">
-        <v>0.8998645612965847</v>
+        <v>0.9034958676589241</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85">
-        <v>1523.936194762405</v>
+        <v>1405.959776283839</v>
       </c>
       <c r="B85">
-        <v>39.0376253729963</v>
+        <v>37.49613015077474</v>
       </c>
       <c r="C85">
-        <v>0.8939890748355164</v>
+        <v>0.9036732984532275</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86">
-        <v>1334.017144031227</v>
+        <v>1407.230428448697</v>
       </c>
       <c r="B86">
-        <v>36.52419943039446</v>
+        <v>37.51307010161521</v>
       </c>
       <c r="C86">
-        <v>0.8882844769150953</v>
+        <v>0.904490003491571</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87">
-        <v>1691.171456220442</v>
+        <v>1407.124386446747</v>
       </c>
       <c r="B87">
-        <v>41.12385507488862</v>
+        <v>37.51165667424923</v>
       </c>
       <c r="C87">
-        <v>0.8930486884439331</v>
+        <v>0.9044218455490033</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88">
-        <v>1510.927180295637</v>
+        <v>1407.338826028491</v>
       </c>
       <c r="B88">
-        <v>38.87064676971091</v>
+        <v>37.51451487129336</v>
       </c>
       <c r="C88">
-        <v>0.8945638488088939</v>
+        <v>0.9045596754694818</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89">
-        <v>1291.579776811522</v>
+        <v>1404.643217609408</v>
       </c>
       <c r="B89">
-        <v>35.93855557491873</v>
+        <v>37.47857011159054</v>
       </c>
       <c r="C89">
-        <v>0.9105639397243628</v>
+        <v>0.9028270872457679</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90">
-        <v>1359.919437972563</v>
+        <v>1404.075215622734</v>
       </c>
       <c r="B90">
-        <v>36.87708554065198</v>
+        <v>37.4709916551822</v>
       </c>
       <c r="C90">
-        <v>0.886631464952463</v>
+        <v>0.9024620069372934</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91">
-        <v>1388.544635147719</v>
+        <v>1405.855823356259</v>
       </c>
       <c r="B91">
-        <v>37.26318069016276</v>
+        <v>37.49474394306834</v>
       </c>
       <c r="C91">
-        <v>0.9050857665993592</v>
+        <v>0.903606483252299</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92">
-        <v>1366.570964966301</v>
+        <v>1404.798044984692</v>
       </c>
       <c r="B92">
-        <v>36.96716062894608</v>
+        <v>37.48063560006276</v>
       </c>
       <c r="C92">
-        <v>0.8825755757026559</v>
+        <v>0.9029266017320787</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93">
-        <v>1349.600931712632</v>
+        <v>1407.088679177757</v>
       </c>
       <c r="B93">
-        <v>36.73691510881979</v>
+        <v>37.51118072225609</v>
       </c>
       <c r="C93">
-        <v>0.9149030976944652</v>
+        <v>0.9043988948884731</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94">
-        <v>1389.896737059011</v>
+        <v>1405.305646239642</v>
       </c>
       <c r="B94">
-        <v>37.28131887499437</v>
+        <v>37.48740650191264</v>
       </c>
       <c r="C94">
-        <v>0.9072655254439318</v>
+        <v>0.903252859785892</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95">
-        <v>1403.294329393171</v>
+        <v>1407.702195050542</v>
       </c>
       <c r="B95">
-        <v>37.46057032925648</v>
+        <v>37.51935760444923</v>
       </c>
       <c r="C95">
-        <v>0.9043523467069765</v>
+        <v>0.9047932290093919</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96">
-        <v>1380.641601172862</v>
+        <v>1407.924566710288</v>
       </c>
       <c r="B96">
-        <v>37.15698590000085</v>
+        <v>37.52232091316164</v>
       </c>
       <c r="C96">
-        <v>0.8993263099590854</v>
+        <v>0.9049361572315435</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97">
-        <v>1503.628785045168</v>
+        <v>1406.75479878788</v>
       </c>
       <c r="B97">
-        <v>38.77665257658489</v>
+        <v>37.50673004659137</v>
       </c>
       <c r="C97">
-        <v>0.8927481358143159</v>
+        <v>0.9041842950127885</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98">
-        <v>1383.150128434909</v>
+        <v>1405.611485491915</v>
       </c>
       <c r="B98">
-        <v>37.19072637681212</v>
+        <v>37.49148550660423</v>
       </c>
       <c r="C98">
-        <v>0.8960260116070179</v>
+        <v>0.9034494363669417</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99">
-        <v>1447.412846768791</v>
+        <v>1404.773165324831</v>
       </c>
       <c r="B99">
-        <v>38.04487937645211</v>
+        <v>37.48030369840713</v>
       </c>
       <c r="C99">
-        <v>0.8956269416445368</v>
+        <v>0.9029106104607288</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100">
-        <v>1384.512286788789</v>
+        <v>1404.122374297765</v>
       </c>
       <c r="B100">
-        <v>37.20903501555487</v>
+        <v>37.47162091900702</v>
       </c>
       <c r="C100">
-        <v>0.9007235976594856</v>
+        <v>0.9024923179292107</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101">
-        <v>1519.635699233669</v>
+        <v>1405.671614969324</v>
       </c>
       <c r="B101">
-        <v>38.98250504051361</v>
+        <v>37.49228740646967</v>
       </c>
       <c r="C101">
-        <v>0.8931943189823305</v>
+        <v>0.9034880842742889</v>
       </c>
     </row>
   </sheetData>
@@ -1499,1102 +1499,1102 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>174.994709119103</v>
+        <v>201.6537963607085</v>
       </c>
       <c r="B2">
-        <v>13.22855657731043</v>
+        <v>14.20048577903969</v>
       </c>
       <c r="C2">
-        <v>0.127673950009389</v>
+        <v>0.1296119237383585</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>199.730845720761</v>
+        <v>204.3477819592056</v>
       </c>
       <c r="B3">
-        <v>14.13261637916918</v>
+        <v>14.29502647633804</v>
       </c>
       <c r="C3">
-        <v>0.1439706726235214</v>
+        <v>0.1313434689026272</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>168.1892670960816</v>
+        <v>206.0161195356951</v>
       </c>
       <c r="B4">
-        <v>12.96878047836733</v>
+        <v>14.35326163405709</v>
       </c>
       <c r="C4">
-        <v>0.1066619410362635</v>
+        <v>0.1324157841609377</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>197.1049822061191</v>
+        <v>209.6401199382716</v>
       </c>
       <c r="B5">
-        <v>14.03940818575053</v>
+        <v>14.47895438000519</v>
       </c>
       <c r="C5">
-        <v>0.124630201297762</v>
+        <v>0.1347450914801327</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>220.2108307568438</v>
+        <v>197.8771784165325</v>
       </c>
       <c r="B6">
-        <v>14.83950237564737</v>
+        <v>14.06688232752846</v>
       </c>
       <c r="C6">
-        <v>0.1312069832536706</v>
+        <v>0.1271845222919032</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>191.2618217212381</v>
+        <v>204.7508017418143</v>
       </c>
       <c r="B7">
-        <v>13.82974409456799</v>
+        <v>14.30911603635299</v>
       </c>
       <c r="C7">
-        <v>0.1349685555925651</v>
+        <v>0.1316025077616582</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>221.0250908749329</v>
+        <v>197.7984783682233</v>
       </c>
       <c r="B8">
-        <v>14.86691262081448</v>
+        <v>14.06408469713629</v>
       </c>
       <c r="C8">
-        <v>0.1343466449144944</v>
+        <v>0.1271339382471501</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>193.4907554347826</v>
+        <v>203.2951022329576</v>
       </c>
       <c r="B9">
-        <v>13.91009545023982</v>
+        <v>14.25815914601031</v>
       </c>
       <c r="C9">
-        <v>0.1234023251544144</v>
+        <v>0.1306668645100408</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>172.0700826444802</v>
+        <v>213.2969656602255</v>
       </c>
       <c r="B10">
-        <v>13.11754865226275</v>
+        <v>14.60468985155883</v>
       </c>
       <c r="C10">
-        <v>0.1054294565610115</v>
+        <v>0.1370955099567041</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>180.1569167591102</v>
+        <v>204.3131721604938</v>
       </c>
       <c r="B11">
-        <v>13.42225453339007</v>
+        <v>14.29381587122536</v>
       </c>
       <c r="C11">
-        <v>0.1363276468040267</v>
+        <v>0.1313212236353814</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>185.368424691358</v>
+        <v>207.9718463553409</v>
       </c>
       <c r="B12">
-        <v>13.61500733350364</v>
+        <v>14.42122901681202</v>
       </c>
       <c r="C12">
-        <v>0.127707711678551</v>
+        <v>0.1336728173533489</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>197.6936520605952</v>
+        <v>208.9444321631777</v>
       </c>
       <c r="B13">
-        <v>14.06035746560504</v>
+        <v>14.45491031321805</v>
       </c>
       <c r="C13">
-        <v>0.1170889862185049</v>
+        <v>0.1342979417984577</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>221.0646397984136</v>
+        <v>214.3773267606012</v>
       </c>
       <c r="B14">
-        <v>14.86824266005951</v>
+        <v>14.64162992158323</v>
       </c>
       <c r="C14">
-        <v>0.1402420986981239</v>
+        <v>0.1377899064078436</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>183.8441785590744</v>
+        <v>200.3248579066023</v>
       </c>
       <c r="B15">
-        <v>13.55891509520855</v>
+        <v>14.15361642502022</v>
       </c>
       <c r="C15">
-        <v>0.1278440730395665</v>
+        <v>0.1287577554922114</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>172.606558191686</v>
+        <v>204.4764029817499</v>
       </c>
       <c r="B16">
-        <v>13.13798151131619</v>
+        <v>14.29952457187825</v>
       </c>
       <c r="C16">
-        <v>0.1297851984626655</v>
+        <v>0.1314261393926749</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>203.647797023916</v>
+        <v>202.1888731964573</v>
       </c>
       <c r="B17">
-        <v>14.27052196045807</v>
+        <v>14.21931338695569</v>
       </c>
       <c r="C17">
-        <v>0.1240289085743781</v>
+        <v>0.1299558415781465</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>202.4588915727321</v>
+        <v>205.8636012238325</v>
       </c>
       <c r="B18">
-        <v>14.22880499454301</v>
+        <v>14.3479476310667</v>
       </c>
       <c r="C18">
-        <v>0.1280190174392972</v>
+        <v>0.1323177538130713</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>210.682055585376</v>
+        <v>204.9981785238862</v>
       </c>
       <c r="B19">
-        <v>14.5148908223719</v>
+        <v>14.31775745443001</v>
       </c>
       <c r="C19">
-        <v>0.1370719872371927</v>
+        <v>0.1317615078955078</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>226.3682524542255</v>
+        <v>205.209859127751</v>
       </c>
       <c r="B20">
-        <v>15.04553928758373</v>
+        <v>14.32514778729179</v>
       </c>
       <c r="C20">
-        <v>0.1410801297406709</v>
+        <v>0.1318975644973686</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>161.1641557642989</v>
+        <v>202.1566377079978</v>
       </c>
       <c r="B21">
-        <v>12.69504453573515</v>
+        <v>14.21817983104722</v>
       </c>
       <c r="C21">
-        <v>0.1042721718569138</v>
+        <v>0.1299351223864059</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>191.9198261227411</v>
+        <v>206.3923167310789</v>
       </c>
       <c r="B22">
-        <v>13.85351313287504</v>
+        <v>14.3663605944957</v>
       </c>
       <c r="C22">
-        <v>0.1141854616118746</v>
+        <v>0.1326575829422088</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>210.8433138665235</v>
+        <v>200.1655972463768</v>
       </c>
       <c r="B23">
-        <v>14.52044468556399</v>
+        <v>14.14798915911292</v>
       </c>
       <c r="C23">
-        <v>0.1443870530104998</v>
+        <v>0.1286553915351701</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>191.9339411462993</v>
+        <v>207.809423236715</v>
       </c>
       <c r="B24">
-        <v>13.854022561924</v>
+        <v>14.41559652725877</v>
       </c>
       <c r="C24">
-        <v>0.1223566166762535</v>
+        <v>0.1335684207426979</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>229.0257405260333</v>
+        <v>200.2860008105206</v>
       </c>
       <c r="B25">
-        <v>15.13359641744266</v>
+        <v>14.15224366701339</v>
       </c>
       <c r="C25">
-        <v>0.1527523482744165</v>
+        <v>0.1287327802967775</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>200.9764968807777</v>
+        <v>203.8764339237788</v>
       </c>
       <c r="B26">
-        <v>14.17661796342053</v>
+        <v>14.27853052396425</v>
       </c>
       <c r="C26">
-        <v>0.1331386268268811</v>
+        <v>0.1310405124161914</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>225.0296877557106</v>
+        <v>216.5890104079442</v>
       </c>
       <c r="B27">
-        <v>15.00098955921611</v>
+        <v>14.71696335552767</v>
       </c>
       <c r="C27">
-        <v>0.1464999385526845</v>
+        <v>0.1392114545135884</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>206.0218400966184</v>
+        <v>201.4241662587225</v>
       </c>
       <c r="B28">
-        <v>14.35346091005993</v>
+        <v>14.19239818560354</v>
       </c>
       <c r="C28">
-        <v>0.1334011443262339</v>
+        <v>0.1294643301903886</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>194.5938427327488</v>
+        <v>216.6800772866344</v>
       </c>
       <c r="B29">
-        <v>13.94968970023164</v>
+        <v>14.72005697294119</v>
       </c>
       <c r="C29">
-        <v>0.1182517147085217</v>
+        <v>0.1392699872739377</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>233.7937921512495</v>
+        <v>199.4238289023081</v>
       </c>
       <c r="B30">
-        <v>15.29031694083708</v>
+        <v>14.12175020676644</v>
       </c>
       <c r="C30">
-        <v>0.1520332570526858</v>
+        <v>0.1281786238086108</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>232.5804241605535</v>
+        <v>206.6869464304885</v>
       </c>
       <c r="B31">
-        <v>15.2505876660722</v>
+        <v>14.37661108990879</v>
       </c>
       <c r="C31">
-        <v>0.1367146687363392</v>
+        <v>0.1328469546417264</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>221.4002334466512</v>
+        <v>206.4043595866881</v>
       </c>
       <c r="B32">
-        <v>14.87952396572724</v>
+        <v>14.36677972221639</v>
       </c>
       <c r="C32">
-        <v>0.1524559755830383</v>
+        <v>0.1326653234247132</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>216.1283759825848</v>
+        <v>206.546260770263</v>
       </c>
       <c r="B33">
-        <v>14.70130524758209</v>
+        <v>14.37171739112146</v>
       </c>
       <c r="C33">
-        <v>0.1346606285343913</v>
+        <v>0.13275652966886</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>186.6646771276913</v>
+        <v>209.1584171792807</v>
       </c>
       <c r="B34">
-        <v>13.66252821141429</v>
+        <v>14.46231022967218</v>
       </c>
       <c r="C34">
-        <v>0.117455767745069</v>
+        <v>0.1344354795492422</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>217.1921972565158</v>
+        <v>209.3451461567365</v>
       </c>
       <c r="B35">
-        <v>14.73744201876689</v>
+        <v>14.46876450000955</v>
       </c>
       <c r="C35">
-        <v>0.134147940535529</v>
+        <v>0.1345554986236278</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>163.692891501163</v>
+        <v>201.9632534514224</v>
       </c>
       <c r="B36">
-        <v>12.79425228378599</v>
+        <v>14.21137760568702</v>
       </c>
       <c r="C36">
-        <v>0.1237703371853471</v>
+        <v>0.1298108256661471</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>209.8301472222222</v>
+        <v>209.6301270424047</v>
       </c>
       <c r="B37">
-        <v>14.4855150830829</v>
+        <v>14.47860929241495</v>
       </c>
       <c r="C37">
-        <v>0.1354335467812104</v>
+        <v>0.1347386685985386</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>196.2800990874933</v>
+        <v>206.3781442914654</v>
       </c>
       <c r="B38">
-        <v>14.00999996743374</v>
+        <v>14.36586733516168</v>
       </c>
       <c r="C38">
-        <v>0.1379983208857087</v>
+        <v>0.132648473680713</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>189.9383060416294</v>
+        <v>206.3868366478798</v>
       </c>
       <c r="B39">
-        <v>13.78181069531973</v>
+        <v>14.36616986701326</v>
       </c>
       <c r="C39">
-        <v>0.1250253269124272</v>
+        <v>0.1326540606473711</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>178.8501524244051</v>
+        <v>201.493340566291</v>
       </c>
       <c r="B40">
-        <v>13.37348692093446</v>
+        <v>14.19483499609245</v>
       </c>
       <c r="C40">
-        <v>0.1193336697509865</v>
+        <v>0.1295087916150634</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>191.1947169141767</v>
+        <v>201.4954111486849</v>
       </c>
       <c r="B41">
-        <v>13.8273177772906</v>
+        <v>14.19490793026446</v>
       </c>
       <c r="C41">
-        <v>0.1190893049253171</v>
+        <v>0.1295101224710758</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
-        <v>208.8794489533011</v>
+        <v>205.5265865727321</v>
       </c>
       <c r="B42">
-        <v>14.45266234827691</v>
+        <v>14.33619847005238</v>
       </c>
       <c r="C42">
-        <v>0.1280601349063383</v>
+        <v>0.132101139407366</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43">
-        <v>210.2959801798175</v>
+        <v>202.7611456977993</v>
       </c>
       <c r="B43">
-        <v>14.50158543676578</v>
+        <v>14.23942223890419</v>
       </c>
       <c r="C43">
-        <v>0.1305370780149659</v>
+        <v>0.1303236667376042</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44">
-        <v>224.9479117820719</v>
+        <v>210.2892452415459</v>
       </c>
       <c r="B44">
-        <v>14.99826362556919</v>
+        <v>14.50135322104616</v>
       </c>
       <c r="C44">
-        <v>0.1458969943982629</v>
+        <v>0.1351623133763874</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45">
-        <v>187.0343800441343</v>
+        <v>214.7615855179818</v>
       </c>
       <c r="B45">
-        <v>13.67605133231571</v>
+        <v>14.65474617719399</v>
       </c>
       <c r="C45">
-        <v>0.1103365065712329</v>
+        <v>0.1380368867159567</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46">
-        <v>202.7171352835928</v>
+        <v>210.4697610842727</v>
       </c>
       <c r="B46">
-        <v>14.23787678284908</v>
+        <v>14.50757598926412</v>
       </c>
       <c r="C46">
-        <v>0.1355859546152316</v>
+        <v>0.1352783389908988</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>260.959202170931</v>
+        <v>208.9704087600644</v>
       </c>
       <c r="B47">
-        <v>16.15423171094593</v>
+        <v>14.45580882413933</v>
       </c>
       <c r="C47">
-        <v>0.1543486701452292</v>
+        <v>0.1343146381203492</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>181.0232495914594</v>
+        <v>201.7478811325819</v>
       </c>
       <c r="B48">
-        <v>13.45448808358978</v>
+        <v>14.20379812348028</v>
       </c>
       <c r="C48">
-        <v>0.1227811777935737</v>
+        <v>0.1296723962337805</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49">
-        <v>201.0753306315978</v>
+        <v>205.9846660520666</v>
       </c>
       <c r="B49">
-        <v>14.1801033364217</v>
+        <v>14.35216590107802</v>
       </c>
       <c r="C49">
-        <v>0.1385255124284002</v>
+        <v>0.1323955675987159</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50">
-        <v>196.9076451959205</v>
+        <v>205.1791078904992</v>
       </c>
       <c r="B50">
-        <v>14.0323784582629</v>
+        <v>14.32407441653733</v>
       </c>
       <c r="C50">
-        <v>0.1271837733374669</v>
+        <v>0.1318777993003348</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51">
-        <v>245.230545595515</v>
+        <v>208.9253818035427</v>
       </c>
       <c r="B51">
-        <v>15.65983861971492</v>
+        <v>14.45425134012629</v>
       </c>
       <c r="C51">
-        <v>0.156841491075857</v>
+        <v>0.1342856972793627</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52">
-        <v>200.633881081887</v>
+        <v>206.4201630273752</v>
       </c>
       <c r="B52">
-        <v>14.16452897493902</v>
+        <v>14.36732971109716</v>
       </c>
       <c r="C52">
-        <v>0.1304149768328566</v>
+        <v>0.1326754810036243</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53">
-        <v>210.6985369296833</v>
+        <v>199.8707955662909</v>
       </c>
       <c r="B53">
-        <v>14.51545855044488</v>
+        <v>14.13756681916273</v>
       </c>
       <c r="C53">
-        <v>0.1297786039701103</v>
+        <v>0.1284659092959743</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54">
-        <v>213.971442058806</v>
+        <v>200.2990158266237</v>
       </c>
       <c r="B54">
-        <v>14.62776271542596</v>
+        <v>14.15270348119481</v>
       </c>
       <c r="C54">
-        <v>0.1443864575687835</v>
+        <v>0.1287411456303594</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55">
-        <v>206.841260237371</v>
+        <v>209.3827277267848</v>
       </c>
       <c r="B55">
-        <v>14.38197692382278</v>
+        <v>14.47006315559074</v>
       </c>
       <c r="C55">
-        <v>0.1300994121684401</v>
+        <v>0.1345796539813708</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56">
-        <v>225.2072036500269</v>
+        <v>208.9001852925389</v>
       </c>
       <c r="B56">
-        <v>15.00690519894181</v>
+        <v>14.45337971868652</v>
       </c>
       <c r="C56">
-        <v>0.1288880629499294</v>
+        <v>0.1342695023535955</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57">
-        <v>197.6255594023976</v>
+        <v>211.1764506977993</v>
       </c>
       <c r="B57">
-        <v>14.05793581584429</v>
+        <v>14.5319114605684</v>
       </c>
       <c r="C57">
-        <v>0.1235384295463568</v>
+        <v>0.1357325600467283</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58">
-        <v>223.110254654977</v>
+        <v>204.1641541814278</v>
       </c>
       <c r="B58">
-        <v>14.93687566578021</v>
+        <v>14.28860224729584</v>
       </c>
       <c r="C58">
-        <v>0.1457738312213618</v>
+        <v>0.1312254431081279</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59">
-        <v>205.382915822747</v>
+        <v>201.8103955394525</v>
       </c>
       <c r="B59">
-        <v>14.33118682533819</v>
+        <v>14.20599857593448</v>
       </c>
       <c r="C59">
-        <v>0.1215333928860884</v>
+        <v>0.1297125770420848</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60">
-        <v>198.0319907079382</v>
+        <v>202.7743126945786</v>
       </c>
       <c r="B60">
-        <v>14.07238397386662</v>
+        <v>14.23988457448229</v>
       </c>
       <c r="C60">
-        <v>0.1359202831663296</v>
+        <v>0.1303321297559715</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61">
-        <v>179.7223573865331</v>
+        <v>205.3090833279657</v>
       </c>
       <c r="B61">
-        <v>13.40605674262693</v>
+        <v>14.32861065588585</v>
       </c>
       <c r="C61">
-        <v>0.1210292883496116</v>
+        <v>0.1319613403334945</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62">
-        <v>228.2722600882686</v>
+        <v>212.2117345786366</v>
       </c>
       <c r="B62">
-        <v>15.10868161317422</v>
+        <v>14.56748895927629</v>
       </c>
       <c r="C62">
-        <v>0.1323733671261139</v>
+        <v>0.1363979833505906</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63">
-        <v>216.7462327786724</v>
+        <v>200.7253050644123</v>
       </c>
       <c r="B63">
-        <v>14.72230392223556</v>
+        <v>14.16775582315041</v>
       </c>
       <c r="C63">
-        <v>0.1286484971413403</v>
+        <v>0.1290151408100958</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64">
-        <v>222.1696084675255</v>
+        <v>209.7776643934514</v>
       </c>
       <c r="B64">
-        <v>14.90535502655088</v>
+        <v>14.48370340739728</v>
       </c>
       <c r="C64">
-        <v>0.1196710811675956</v>
+        <v>0.1348334974598718</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65">
-        <v>186.0814785531103</v>
+        <v>212.0982555179818</v>
       </c>
       <c r="B65">
-        <v>13.64116851860977</v>
+        <v>14.56359349604286</v>
       </c>
       <c r="C65">
-        <v>0.1043472805222893</v>
+        <v>0.1363250452774125</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66">
-        <v>199.3553688853104</v>
+        <v>213.3723220075148</v>
       </c>
       <c r="B66">
-        <v>14.11932607758991</v>
+        <v>14.60726949184942</v>
       </c>
       <c r="C66">
-        <v>0.125235899882588</v>
+        <v>0.1371439448551011</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67">
-        <v>226.140557505815</v>
+        <v>209.1848938888889</v>
       </c>
       <c r="B67">
-        <v>15.03797052483529</v>
+        <v>14.46322557000647</v>
       </c>
       <c r="C67">
-        <v>0.1546638548479778</v>
+        <v>0.1344524973159723</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68">
-        <v>196.285829898014</v>
+        <v>210.2825086044015</v>
       </c>
       <c r="B68">
-        <v>14.01020449165586</v>
+        <v>14.50112094303063</v>
       </c>
       <c r="C68">
-        <v>0.1470852848570536</v>
+        <v>0.1351579834380702</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69">
-        <v>213.9230075013419</v>
+        <v>203.7352576221149</v>
       </c>
       <c r="B69">
-        <v>14.62610705216333</v>
+        <v>14.27358601130476</v>
       </c>
       <c r="C69">
-        <v>0.1385813485639185</v>
+        <v>0.1309497720861051</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70">
-        <v>186.2572771470746</v>
+        <v>200.2059959527644</v>
       </c>
       <c r="B70">
-        <v>13.64761067539203</v>
+        <v>14.14941680610068</v>
       </c>
       <c r="C70">
-        <v>0.1078174691535159</v>
+        <v>0.1286813575925737</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71">
-        <v>204.9367849943341</v>
+        <v>204.5977467257112</v>
       </c>
       <c r="B71">
-        <v>14.31561332931056</v>
+        <v>14.30376687190165</v>
       </c>
       <c r="C71">
-        <v>0.1332943629026668</v>
+        <v>0.1315041324499459</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72">
-        <v>220.9478226635653</v>
+        <v>213.135771591519</v>
       </c>
       <c r="B72">
-        <v>14.86431372998987</v>
+        <v>14.5991702364045</v>
       </c>
       <c r="C72">
-        <v>0.1364242843215337</v>
+        <v>0.1369919033114679</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73">
-        <v>229.260243239697</v>
+        <v>209.4482777375202</v>
       </c>
       <c r="B73">
-        <v>15.1413421875241</v>
+        <v>14.4723279999287</v>
       </c>
       <c r="C73">
-        <v>0.1273332550523623</v>
+        <v>0.1346217859081952</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74">
-        <v>233.1673375559134</v>
+        <v>209.9575667579173</v>
       </c>
       <c r="B74">
-        <v>15.26981786256514</v>
+        <v>14.48991258627592</v>
       </c>
       <c r="C74">
-        <v>0.1518792122135883</v>
+        <v>0.1349491287644364</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75">
-        <v>216.9179583601718</v>
+        <v>200.4591555179817</v>
       </c>
       <c r="B75">
-        <v>14.72813492470013</v>
+        <v>14.15835991624672</v>
       </c>
       <c r="C75">
-        <v>0.1276187213634035</v>
+        <v>0.1288440745800653</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76">
-        <v>199.3434116299875</v>
+        <v>208.5301138056897</v>
       </c>
       <c r="B76">
-        <v>14.11890263547375</v>
+        <v>14.44057179635522</v>
       </c>
       <c r="C76">
-        <v>0.1322766554294516</v>
+        <v>0.1340316408394733</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77">
-        <v>166.2070418679549</v>
+        <v>200.5100021685453</v>
       </c>
       <c r="B77">
-        <v>12.89213100569316</v>
+        <v>14.16015544295137</v>
       </c>
       <c r="C77">
-        <v>0.0992603047177586</v>
+        <v>0.1288767559989828</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78">
-        <v>195.8151697560685</v>
+        <v>210.5017092216854</v>
       </c>
       <c r="B78">
-        <v>13.99339736290185</v>
+        <v>14.50867703209653</v>
       </c>
       <c r="C78">
-        <v>0.1221800335893759</v>
+        <v>0.135298873489254</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79">
-        <v>244.4458580515298</v>
+        <v>212.6071956709608</v>
       </c>
       <c r="B79">
-        <v>15.63476440665256</v>
+        <v>14.58105605472254</v>
       </c>
       <c r="C79">
-        <v>0.1419531535563179</v>
+        <v>0.1366521639009441</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80">
-        <v>178.9628800978111</v>
+        <v>212.0329746618358</v>
       </c>
       <c r="B80">
-        <v>13.37770085245634</v>
+        <v>14.56135208906906</v>
       </c>
       <c r="C80">
-        <v>0.1158101373072155</v>
+        <v>0.1362830863482935</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81">
-        <v>196.324150867776</v>
+        <v>199.8176863633924</v>
       </c>
       <c r="B81">
-        <v>14.01157203413578</v>
+        <v>14.13568839368612</v>
       </c>
       <c r="C81">
-        <v>0.1182497662577631</v>
+        <v>0.1284317736333656</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82">
-        <v>223.9978847557703</v>
+        <v>201.6321501529791</v>
       </c>
       <c r="B82">
-        <v>14.96655888157897</v>
+        <v>14.19972359424574</v>
       </c>
       <c r="C82">
-        <v>0.1324240870099128</v>
+        <v>0.129598010751468</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83">
-        <v>204.4958932501342</v>
+        <v>202.0102638325282</v>
       </c>
       <c r="B83">
-        <v>14.30020605621241</v>
+        <v>14.21303147933361</v>
       </c>
       <c r="C83">
-        <v>0.1297382521120197</v>
+        <v>0.1298410413429205</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84">
-        <v>219.9403777106817</v>
+        <v>214.0967795974235</v>
       </c>
       <c r="B84">
-        <v>14.83038697103625</v>
+        <v>14.63204632296602</v>
       </c>
       <c r="C84">
-        <v>0.1459524160537868</v>
+        <v>0.1376095861848928</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85">
-        <v>253.0744705850778</v>
+        <v>208.3934359634997</v>
       </c>
       <c r="B85">
-        <v>15.90831451113152</v>
+        <v>14.43583859578306</v>
       </c>
       <c r="C85">
-        <v>0.1484614727312242</v>
+        <v>0.1339437918707037</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86">
-        <v>167.6493874932904</v>
+        <v>201.9198493961352</v>
       </c>
       <c r="B86">
-        <v>12.94794916167384</v>
+        <v>14.20985043538936</v>
       </c>
       <c r="C86">
-        <v>0.1116330094713741</v>
+        <v>0.1297829279364465</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87">
-        <v>214.4339746824119</v>
+        <v>203.801463475577</v>
       </c>
       <c r="B87">
-        <v>14.64356427521701</v>
+        <v>14.27590499672707</v>
       </c>
       <c r="C87">
-        <v>0.1132351064367684</v>
+        <v>0.1309923255524161</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88">
-        <v>216.7785068348542</v>
+        <v>202.8024841680086</v>
       </c>
       <c r="B88">
-        <v>14.72339997537438</v>
+        <v>14.24087371505023</v>
       </c>
       <c r="C88">
-        <v>0.12834650004462</v>
+        <v>0.1303502368232901</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89">
-        <v>175.6419777360291</v>
+        <v>200.2812467901234</v>
       </c>
       <c r="B89">
-        <v>13.25299882049452</v>
+        <v>14.15207570606247</v>
       </c>
       <c r="C89">
-        <v>0.1238276211037614</v>
+        <v>0.1287297246750128</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90">
-        <v>236.0220934916801</v>
+        <v>201.1658485077832</v>
       </c>
       <c r="B90">
-        <v>15.36301056081392</v>
+        <v>14.1832946986158</v>
       </c>
       <c r="C90">
-        <v>0.1538801554492514</v>
+        <v>0.1292982978059781</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91">
-        <v>203.1530406035665</v>
+        <v>206.4780252200751</v>
       </c>
       <c r="B91">
-        <v>14.25317650924055</v>
+        <v>14.36934324247546</v>
       </c>
       <c r="C91">
-        <v>0.1324198883042085</v>
+        <v>0.1327126716255855</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92">
-        <v>190.5499464424167</v>
+        <v>207.2040757165861</v>
       </c>
       <c r="B92">
-        <v>13.80398299196347</v>
+        <v>14.39458494422768</v>
       </c>
       <c r="C92">
-        <v>0.1230632971085212</v>
+        <v>0.1331793367877713</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93">
-        <v>230.0410804735492</v>
+        <v>204.0543703166935</v>
       </c>
       <c r="B93">
-        <v>15.16710521073646</v>
+        <v>14.28476007207309</v>
       </c>
       <c r="C93">
-        <v>0.1559463187796952</v>
+        <v>0.1311548801028145</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94">
-        <v>210.2772811057434</v>
+        <v>197.1711615995706</v>
       </c>
       <c r="B94">
-        <v>14.50094069727007</v>
+        <v>14.04176490330082</v>
       </c>
       <c r="C94">
-        <v>0.1372600732447246</v>
+        <v>0.1267307336725473</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95">
-        <v>214.3364074342458</v>
+        <v>211.2875988164251</v>
       </c>
       <c r="B95">
-        <v>14.64023249249293</v>
+        <v>14.53573523480753</v>
       </c>
       <c r="C95">
-        <v>0.1381289933179769</v>
+        <v>0.1358039999190983</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96">
-        <v>197.230101425419</v>
+        <v>203.547141062802</v>
       </c>
       <c r="B96">
-        <v>14.04386347930722</v>
+        <v>14.26699481540531</v>
       </c>
       <c r="C96">
-        <v>0.1284723125661995</v>
+        <v>0.1308288611507312</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97">
-        <v>234.6691276734061</v>
+        <v>206.2206532769726</v>
       </c>
       <c r="B97">
-        <v>15.31891405006915</v>
+        <v>14.3603848582471</v>
       </c>
       <c r="C97">
-        <v>0.1393298853728124</v>
+        <v>0.1325472471542197</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98">
-        <v>191.7344966586151</v>
+        <v>214.6278090311326</v>
       </c>
       <c r="B98">
-        <v>13.84682261959816</v>
+        <v>14.65018119448127</v>
       </c>
       <c r="C98">
-        <v>0.1242085676721838</v>
+        <v>0.1379509025781709</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99">
-        <v>204.1623529552096</v>
+        <v>201.8176694229737</v>
       </c>
       <c r="B99">
-        <v>14.2885392169812</v>
+        <v>14.20625458813736</v>
       </c>
       <c r="C99">
-        <v>0.1263311322574132</v>
+        <v>0.1297172522927051</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100">
-        <v>235.033890326236</v>
+        <v>204.8006072007515</v>
       </c>
       <c r="B100">
-        <v>15.33081505746632</v>
+        <v>14.31085627070412</v>
       </c>
       <c r="C100">
-        <v>0.152906242354531</v>
+        <v>0.131634519960099</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101">
-        <v>217.2531168276973</v>
+        <v>213.05321784219</v>
       </c>
       <c r="B101">
-        <v>14.73950870374238</v>
+        <v>14.59634261869014</v>
       </c>
       <c r="C101">
-        <v>0.1276945848465932</v>
+        <v>0.1369388423205239</v>
       </c>
     </row>
   </sheetData>
@@ -2623,1102 +2623,1102 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>182.5185696485665</v>
+        <v>285.2817248632369</v>
       </c>
       <c r="B2">
-        <v>13.50994336215243</v>
+        <v>16.89028492546046</v>
       </c>
       <c r="C2">
-        <v>0.1331632645032493</v>
+        <v>0.183363337731465</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>208.7268324593809</v>
+        <v>311.7662736334639</v>
       </c>
       <c r="B3">
-        <v>14.44738150875033</v>
+        <v>17.65690441820038</v>
       </c>
       <c r="C3">
-        <v>0.1504551906107034</v>
+        <v>0.2003861430413733</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>199.2063973598283</v>
+        <v>291.8971387510454</v>
       </c>
       <c r="B4">
-        <v>14.11404964423139</v>
+        <v>17.08499747588642</v>
       </c>
       <c r="C4">
-        <v>0.1263323241494493</v>
+        <v>0.1876153604347272</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>203.8815825515215</v>
+        <v>291.9100406363696</v>
       </c>
       <c r="B5">
-        <v>14.27871081545955</v>
+        <v>17.08537505108886</v>
       </c>
       <c r="C5">
-        <v>0.128915070486298</v>
+        <v>0.1876236530540915</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>203.3852784551465</v>
+        <v>278.220255490617</v>
       </c>
       <c r="B6">
-        <v>14.26132106276086</v>
+        <v>16.67993571602172</v>
       </c>
       <c r="C6">
-        <v>0.1211819088670233</v>
+        <v>0.1788246151964966</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>203.1704480256988</v>
+        <v>291.8524001560607</v>
       </c>
       <c r="B7">
-        <v>14.25378714677958</v>
+        <v>17.0836881309646</v>
       </c>
       <c r="C7">
-        <v>0.143372167337659</v>
+        <v>0.1875866049366078</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>226.3926455244837</v>
+        <v>287.007344255868</v>
       </c>
       <c r="B8">
-        <v>15.0463499070201</v>
+        <v>16.94129110356906</v>
       </c>
       <c r="C8">
-        <v>0.1376092290659486</v>
+        <v>0.1844724705777373</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>185.6280192897084</v>
+        <v>287.9431478642677</v>
       </c>
       <c r="B9">
-        <v>13.62453739727365</v>
+        <v>16.96888764369273</v>
       </c>
       <c r="C9">
-        <v>0.118387719055029</v>
+        <v>0.1850739534563901</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>183.4006504486829</v>
+        <v>293.5069324913487</v>
       </c>
       <c r="B10">
-        <v>13.54254962880635</v>
+        <v>17.13204402549061</v>
       </c>
       <c r="C10">
-        <v>0.112371834851101</v>
+        <v>0.1886500469482889</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>203.856636393948</v>
+        <v>295.2219904318795</v>
       </c>
       <c r="B11">
-        <v>14.27783724497334</v>
+        <v>17.18202521334082</v>
       </c>
       <c r="C11">
-        <v>0.1542616071862024</v>
+        <v>0.1897523914764162</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>220.6663957461095</v>
+        <v>323.0829582469126</v>
       </c>
       <c r="B12">
-        <v>14.85484418451131</v>
+        <v>17.97450856760519</v>
       </c>
       <c r="C12">
-        <v>0.1520258937950768</v>
+        <v>0.2076598829340004</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>200.4089703180277</v>
+        <v>294.3371361294732</v>
       </c>
       <c r="B13">
-        <v>14.15658752376531</v>
+        <v>17.15625647189599</v>
       </c>
       <c r="C13">
-        <v>0.1186972010433594</v>
+        <v>0.1891836559979254</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>211.9617396012917</v>
+        <v>294.8078341920026</v>
       </c>
       <c r="B14">
-        <v>14.55890585179023</v>
+        <v>17.16996896304716</v>
       </c>
       <c r="C14">
-        <v>0.1344672727058349</v>
+        <v>0.1894861947176766</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>210.3207979468469</v>
+        <v>299.2273244277114</v>
       </c>
       <c r="B15">
-        <v>14.50244110302975</v>
+        <v>17.29818847243004</v>
       </c>
       <c r="C15">
-        <v>0.1462557458452062</v>
+        <v>0.1923267989697733</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>170.9120822719799</v>
+        <v>269.3489247983716</v>
       </c>
       <c r="B16">
-        <v>13.07333478007734</v>
+        <v>16.41185317989323</v>
       </c>
       <c r="C16">
-        <v>0.1285110991709974</v>
+        <v>0.1731226137569388</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>195.986398427819</v>
+        <v>304.7662195967954</v>
       </c>
       <c r="B17">
-        <v>13.99951422113707</v>
+        <v>17.45755480005133</v>
       </c>
       <c r="C17">
-        <v>0.1193628384282055</v>
+        <v>0.1958868948926186</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>196.7268714215018</v>
+        <v>327.3722967237794</v>
       </c>
       <c r="B18">
-        <v>14.02593567008996</v>
+        <v>18.0934324196317</v>
       </c>
       <c r="C18">
-        <v>0.1243945404800373</v>
+        <v>0.2104168328232928</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>199.2735876051474</v>
+        <v>307.6358023095025</v>
       </c>
       <c r="B19">
-        <v>14.11642970460829</v>
+        <v>17.53954966096628</v>
       </c>
       <c r="C19">
-        <v>0.129649516571446</v>
+        <v>0.1977313041843478</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>244.2237836725666</v>
+        <v>298.1585621477264</v>
       </c>
       <c r="B20">
-        <v>15.62766085095804</v>
+        <v>17.2672685201721</v>
       </c>
       <c r="C20">
-        <v>0.1522082832408259</v>
+        <v>0.1916398575998212</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>182.8920414303128</v>
+        <v>329.2600735181449</v>
       </c>
       <c r="B21">
-        <v>13.52375840623873</v>
+        <v>18.14552488957387</v>
       </c>
       <c r="C21">
-        <v>0.1183299740866321</v>
+        <v>0.2116301914920707</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>203.2481274254629</v>
+        <v>293.5579419551821</v>
       </c>
       <c r="B22">
-        <v>14.2565117551757</v>
+        <v>17.13353267587225</v>
       </c>
       <c r="C22">
-        <v>0.1209253974468646</v>
+        <v>0.1886828330145814</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>214.5961053651224</v>
+        <v>287.010132591472</v>
       </c>
       <c r="B23">
-        <v>14.64909913152077</v>
+        <v>16.94137339743954</v>
       </c>
       <c r="C23">
-        <v>0.1469569922469355</v>
+        <v>0.1844742627658739</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>192.8917801511155</v>
+        <v>287.5257652749555</v>
       </c>
       <c r="B24">
-        <v>13.88854852571411</v>
+        <v>16.95658471729952</v>
       </c>
       <c r="C24">
-        <v>0.122967232699923</v>
+        <v>0.1848056829784121</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>217.6173619951863</v>
+        <v>299.4736390164231</v>
       </c>
       <c r="B25">
-        <v>14.7518596114248</v>
+        <v>17.30530667212873</v>
       </c>
       <c r="C25">
-        <v>0.1451433493619463</v>
+        <v>0.1924851163843906</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>201.7857788167731</v>
+        <v>300.9355445199701</v>
       </c>
       <c r="B26">
-        <v>14.20513212950774</v>
+        <v>17.34749389738962</v>
       </c>
       <c r="C26">
-        <v>0.1336747426779714</v>
+        <v>0.1934247485066595</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>239.2520580744424</v>
+        <v>289.4255351342498</v>
       </c>
       <c r="B27">
-        <v>15.46777482621345</v>
+        <v>17.01251113546292</v>
       </c>
       <c r="C27">
-        <v>0.1557590563097589</v>
+        <v>0.1860267501269966</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>205.0142846119443</v>
+        <v>287.8377697526805</v>
       </c>
       <c r="B28">
-        <v>14.31831989487399</v>
+        <v>16.96578232067948</v>
       </c>
       <c r="C28">
-        <v>0.1327487423548475</v>
+        <v>0.1850062222258888</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>207.7491951206524</v>
+        <v>306.9083792045575</v>
       </c>
       <c r="B29">
-        <v>14.41350738441731</v>
+        <v>17.51880073534023</v>
       </c>
       <c r="C29">
-        <v>0.1262460220083733</v>
+        <v>0.197263756785265</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>228.2848286732144</v>
+        <v>288.9424849077001</v>
       </c>
       <c r="B30">
-        <v>15.10909754661788</v>
+        <v>16.99830829546576</v>
       </c>
       <c r="C30">
-        <v>0.1484508451638021</v>
+        <v>0.1857162721183709</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>248.9220393073085</v>
+        <v>301.3881832493845</v>
       </c>
       <c r="B31">
-        <v>15.77726336559381</v>
+        <v>17.36053522358641</v>
       </c>
       <c r="C31">
-        <v>0.1463205438200623</v>
+        <v>0.1937156796844373</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>222.1695404952892</v>
+        <v>311.0043062912287</v>
       </c>
       <c r="B32">
-        <v>14.90535274642265</v>
+        <v>17.63531418181226</v>
       </c>
       <c r="C32">
-        <v>0.1529857196343306</v>
+        <v>0.1998963925143042</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>211.6192618451662</v>
+        <v>306.03303792463</v>
       </c>
       <c r="B33">
-        <v>14.54713930108481</v>
+        <v>17.49379998526992</v>
       </c>
       <c r="C33">
-        <v>0.1318511865019995</v>
+        <v>0.1967011357522527</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>186.1404866165059</v>
+        <v>284.3890619059699</v>
       </c>
       <c r="B34">
-        <v>13.64333121405861</v>
+        <v>16.86383888401362</v>
       </c>
       <c r="C34">
-        <v>0.1171259292352698</v>
+        <v>0.1827895832808722</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>201.9313685647986</v>
+        <v>328.2174947914202</v>
       </c>
       <c r="B35">
-        <v>14.21025575296935</v>
+        <v>18.11677385163871</v>
       </c>
       <c r="C35">
-        <v>0.1247221473177311</v>
+        <v>0.2109600794641387</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>176.9551543279596</v>
+        <v>292.3899082748089</v>
       </c>
       <c r="B36">
-        <v>13.3024491853177</v>
+        <v>17.09941251256338</v>
       </c>
       <c r="C36">
-        <v>0.1337981076453843</v>
+        <v>0.1879320854708415</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>225.9304865081029</v>
+        <v>294.9704943023638</v>
       </c>
       <c r="B37">
-        <v>15.03098421621495</v>
+        <v>17.17470507177238</v>
       </c>
       <c r="C37">
-        <v>0.1458254093554588</v>
+        <v>0.1895907436535272</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>190.1009489607674</v>
+        <v>303.6376849733845</v>
       </c>
       <c r="B38">
-        <v>13.78771006950637</v>
+        <v>17.42520258055511</v>
       </c>
       <c r="C38">
-        <v>0.1336539561439285</v>
+        <v>0.1951615351613083</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>186.7780036362888</v>
+        <v>289.6140091464313</v>
       </c>
       <c r="B39">
-        <v>13.66667492978043</v>
+        <v>17.01804951063521</v>
       </c>
       <c r="C39">
-        <v>0.1229450838608586</v>
+        <v>0.1861478908133347</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>199.5770369314239</v>
+        <v>302.4188442700715</v>
       </c>
       <c r="B40">
-        <v>14.1271737064221</v>
+        <v>17.39019391122685</v>
       </c>
       <c r="C40">
-        <v>0.1331632089333635</v>
+        <v>0.1943781316690937</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>201.3842110341228</v>
+        <v>304.256122683404</v>
       </c>
       <c r="B41">
-        <v>14.19099048812742</v>
+        <v>17.44293904946652</v>
       </c>
       <c r="C41">
-        <v>0.1254360272190598</v>
+        <v>0.1955590327673798</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
-        <v>217.9769157063175</v>
+        <v>285.5921631432632</v>
       </c>
       <c r="B42">
-        <v>14.76404130671265</v>
+        <v>16.89947227410558</v>
       </c>
       <c r="C42">
-        <v>0.1336376238624581</v>
+        <v>0.1835628703135556</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43">
-        <v>228.7416533941727</v>
+        <v>300.7729911081622</v>
       </c>
       <c r="B43">
-        <v>15.12420752945994</v>
+        <v>17.34280805141319</v>
       </c>
       <c r="C43">
-        <v>0.1419868655066802</v>
+        <v>0.1933202681507515</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44">
-        <v>214.5173422721904</v>
+        <v>295.8526434859706</v>
       </c>
       <c r="B44">
-        <v>14.64641055932102</v>
+        <v>17.20036753926993</v>
       </c>
       <c r="C44">
-        <v>0.1391319227454613</v>
+        <v>0.1901577404310466</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45">
-        <v>188.4991283329906</v>
+        <v>317.2784743507285</v>
       </c>
       <c r="B45">
-        <v>13.72949847346911</v>
+        <v>17.81231243692768</v>
       </c>
       <c r="C45">
-        <v>0.1112006001627992</v>
+        <v>0.2039290812448181</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46">
-        <v>225.410559646604</v>
+        <v>291.5387791206491</v>
       </c>
       <c r="B46">
-        <v>15.01367908430855</v>
+        <v>17.07450670211731</v>
       </c>
       <c r="C46">
-        <v>0.150764294627994</v>
+        <v>0.187385026655129</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>257.4417551470248</v>
+        <v>296.2010595587437</v>
       </c>
       <c r="B47">
-        <v>16.04499159074335</v>
+        <v>17.21049271690801</v>
       </c>
       <c r="C47">
-        <v>0.1522682174693716</v>
+        <v>0.1903816830409503</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>205.3820546609956</v>
+        <v>281.9003486961192</v>
       </c>
       <c r="B48">
-        <v>14.33115678028105</v>
+        <v>16.78988828718402</v>
       </c>
       <c r="C48">
-        <v>0.1393028278182611</v>
+        <v>0.1811899758716213</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49">
-        <v>190.1200560622669</v>
+        <v>291.4474815047742</v>
       </c>
       <c r="B49">
-        <v>13.78840295546467</v>
+        <v>17.07183298608483</v>
       </c>
       <c r="C49">
-        <v>0.1309781667707134</v>
+        <v>0.1873263455896617</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50">
-        <v>198.5868123442152</v>
+        <v>288.6249400492928</v>
       </c>
       <c r="B50">
-        <v>14.09208332164607</v>
+        <v>16.98896524363073</v>
       </c>
       <c r="C50">
-        <v>0.1282683569948055</v>
+        <v>0.1855121718201664</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51">
-        <v>235.9512584740123</v>
+        <v>297.817178403856</v>
       </c>
       <c r="B51">
-        <v>15.36070501227116</v>
+        <v>17.25738040386941</v>
       </c>
       <c r="C51">
-        <v>0.1509067604544211</v>
+        <v>0.1914204349825712</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52">
-        <v>200.4730275702943</v>
+        <v>288.0850276682983</v>
       </c>
       <c r="B52">
-        <v>14.15884979686889</v>
+        <v>16.9730677153041</v>
       </c>
       <c r="C52">
-        <v>0.1303104196819171</v>
+        <v>0.1851651459589461</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53">
-        <v>213.2692944834077</v>
+        <v>287.4262389121374</v>
       </c>
       <c r="B53">
-        <v>14.60374248209711</v>
+        <v>16.95364972246794</v>
       </c>
       <c r="C53">
-        <v>0.1313620479338404</v>
+        <v>0.1847417129288492</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54">
-        <v>216.3131328096194</v>
+        <v>275.0759810675901</v>
       </c>
       <c r="B54">
-        <v>14.70758759313095</v>
+        <v>16.58541470894201</v>
       </c>
       <c r="C54">
-        <v>0.1459666143830678</v>
+        <v>0.1768036492435378</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55">
-        <v>213.1757764085646</v>
+        <v>295.0251892136626</v>
       </c>
       <c r="B55">
-        <v>14.60054027796796</v>
+        <v>17.17629730802487</v>
       </c>
       <c r="C55">
-        <v>0.1340837082866235</v>
+        <v>0.1896258985219211</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56">
-        <v>247.9169250738691</v>
+        <v>287.1180717844364</v>
       </c>
       <c r="B56">
-        <v>15.74537789555618</v>
+        <v>16.94455876629534</v>
       </c>
       <c r="C56">
-        <v>0.1418850362128277</v>
+        <v>0.1845436401180498</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57">
-        <v>219.2302705861771</v>
+        <v>295.5008639106811</v>
       </c>
       <c r="B57">
-        <v>14.8064266650052</v>
+        <v>17.19013856577896</v>
       </c>
       <c r="C57">
-        <v>0.1370438288404451</v>
+        <v>0.1899316359474826</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58">
-        <v>217.7202902259086</v>
+        <v>300.0482741474847</v>
       </c>
       <c r="B58">
-        <v>14.75534785174204</v>
+        <v>17.32190157423499</v>
       </c>
       <c r="C58">
-        <v>0.1422521832980642</v>
+        <v>0.1928544601117521</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59">
-        <v>223.4222518807892</v>
+        <v>289.6904077854642</v>
       </c>
       <c r="B59">
-        <v>14.94731587546036</v>
+        <v>17.02029399820885</v>
       </c>
       <c r="C59">
-        <v>0.1322079989396831</v>
+        <v>0.1861969956393014</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60">
-        <v>202.4590135388688</v>
+        <v>285.1496842230895</v>
       </c>
       <c r="B60">
-        <v>14.22880928043063</v>
+        <v>16.88637569826899</v>
       </c>
       <c r="C60">
-        <v>0.1389587932303505</v>
+        <v>0.1832784693000757</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61">
-        <v>170.2542294217336</v>
+        <v>308.0459803811265</v>
       </c>
       <c r="B61">
-        <v>13.04815042148632</v>
+        <v>17.55123871358163</v>
       </c>
       <c r="C61">
-        <v>0.1146532269277263</v>
+        <v>0.1979949439962294</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62">
-        <v>238.5461642461561</v>
+        <v>300.9155862374959</v>
       </c>
       <c r="B62">
-        <v>15.44493976181701</v>
+        <v>17.34691863811829</v>
       </c>
       <c r="C62">
-        <v>0.1383311268923896</v>
+        <v>0.193411920424905</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63">
-        <v>230.2176183928903</v>
+        <v>309.8894003706987</v>
       </c>
       <c r="B63">
-        <v>15.17292385774378</v>
+        <v>17.60367576305297</v>
       </c>
       <c r="C63">
-        <v>0.1366443616667026</v>
+        <v>0.1991797925605447</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64">
-        <v>239.5116452186462</v>
+        <v>304.095147238846</v>
       </c>
       <c r="B64">
-        <v>15.47616377590539</v>
+        <v>17.43832409490218</v>
       </c>
       <c r="C64">
-        <v>0.1290123241124334</v>
+        <v>0.1954555666416673</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65">
-        <v>191.205163966041</v>
+        <v>288.8093288266234</v>
       </c>
       <c r="B65">
-        <v>13.82769554069083</v>
+        <v>16.9943910990251</v>
       </c>
       <c r="C65">
-        <v>0.1072204447041752</v>
+        <v>0.1856306867431532</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66">
-        <v>193.3981462113414</v>
+        <v>290.8273423593352</v>
       </c>
       <c r="B66">
-        <v>13.90676620251241</v>
+        <v>17.05366067327878</v>
       </c>
       <c r="C66">
-        <v>0.1214935469851115</v>
+        <v>0.1869277543948688</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67">
-        <v>212.4047426156948</v>
+        <v>294.3395317139658</v>
       </c>
       <c r="B67">
-        <v>14.57411206954629</v>
+        <v>17.15632628839769</v>
       </c>
       <c r="C67">
-        <v>0.1452695467069921</v>
+        <v>0.1891851957473394</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68">
-        <v>183.2407398228654</v>
+        <v>301.5840432726169</v>
       </c>
       <c r="B68">
-        <v>13.53664433391324</v>
+        <v>17.36617526321259</v>
       </c>
       <c r="C68">
-        <v>0.1373100464168363</v>
+        <v>0.1938415676907728</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69">
-        <v>201.6619907372602</v>
+        <v>302.7799639498537</v>
       </c>
       <c r="B69">
-        <v>14.2007743006239</v>
+        <v>17.40057366726321</v>
       </c>
       <c r="C69">
-        <v>0.1306385458809458</v>
+        <v>0.1946102394560094</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70">
-        <v>199.1082637867569</v>
+        <v>272.2995957475322</v>
       </c>
       <c r="B70">
-        <v>14.11057276607711</v>
+        <v>16.50150283300076</v>
       </c>
       <c r="C70">
-        <v>0.1152564314149579</v>
+        <v>0.1750191420888675</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71">
-        <v>197.4696191335003</v>
+        <v>280.0348383607827</v>
       </c>
       <c r="B71">
-        <v>14.05238837826155</v>
+        <v>16.73424149344041</v>
       </c>
       <c r="C71">
-        <v>0.1284375915029601</v>
+        <v>0.179990928853015</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72">
-        <v>227.8920035957156</v>
+        <v>302.7485267939001</v>
       </c>
       <c r="B72">
-        <v>15.09609232866955</v>
+        <v>17.39967030704605</v>
       </c>
       <c r="C72">
-        <v>0.1407119704478222</v>
+        <v>0.1945900333883163</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73">
-        <v>221.0758638510817</v>
+        <v>281.0766601360265</v>
       </c>
       <c r="B73">
-        <v>14.8686201058162</v>
+        <v>16.76534103846464</v>
       </c>
       <c r="C73">
-        <v>0.12278757520221</v>
+        <v>0.1806605543543403</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74">
-        <v>223.8910388460252</v>
+        <v>282.1472595733342</v>
       </c>
       <c r="B74">
-        <v>14.96298896765032</v>
+        <v>16.79723964148081</v>
       </c>
       <c r="C74">
-        <v>0.1458368695978362</v>
+        <v>0.1813486765475568</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75">
-        <v>260.1379449759419</v>
+        <v>286.0618740350399</v>
       </c>
       <c r="B75">
-        <v>16.12879242150329</v>
+        <v>16.91336377055256</v>
       </c>
       <c r="C75">
-        <v>0.1530462123417655</v>
+        <v>0.1838647745344688</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76">
-        <v>190.1961257977384</v>
+        <v>286.1262987781531</v>
       </c>
       <c r="B76">
-        <v>13.79116114755166</v>
+        <v>16.9152682147861</v>
       </c>
       <c r="C76">
-        <v>0.1262068667855566</v>
+        <v>0.1839061832014115</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77">
-        <v>186.9759139549848</v>
+        <v>298.2015078044705</v>
       </c>
       <c r="B77">
-        <v>13.67391362979103</v>
+        <v>17.26851203214888</v>
       </c>
       <c r="C77">
-        <v>0.1116636574808778</v>
+        <v>0.1916674606962518</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78">
-        <v>193.5588553365619</v>
+        <v>299.546330437734</v>
       </c>
       <c r="B78">
-        <v>13.91254309378993</v>
+        <v>17.30740680858152</v>
       </c>
       <c r="C78">
-        <v>0.1207721928592279</v>
+        <v>0.1925318384155427</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79">
-        <v>229.7688773228146</v>
+        <v>322.3131915827762</v>
       </c>
       <c r="B79">
-        <v>15.15812908385512</v>
+        <v>17.95308306622504</v>
       </c>
       <c r="C79">
-        <v>0.1334300240758938</v>
+        <v>0.2071651194335427</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80">
-        <v>199.8089687344448</v>
+        <v>283.9499055008229</v>
       </c>
       <c r="B80">
-        <v>14.1353800350201</v>
+        <v>16.85081319998601</v>
       </c>
       <c r="C80">
-        <v>0.1293000207177168</v>
+        <v>0.1825073177965593</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81">
-        <v>203.5674201474639</v>
+        <v>301.5134132442357</v>
       </c>
       <c r="B81">
-        <v>14.26770549694182</v>
+        <v>17.3641415924956</v>
       </c>
       <c r="C81">
-        <v>0.1226125249681881</v>
+        <v>0.1937961706091544</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82">
-        <v>244.4202113009226</v>
+        <v>288.383810828885</v>
       </c>
       <c r="B82">
-        <v>15.63394420166973</v>
+        <v>16.98186711845565</v>
       </c>
       <c r="C82">
-        <v>0.1444974507843478</v>
+        <v>0.1853571872739287</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83">
-        <v>211.872930897431</v>
+        <v>296.5188743740133</v>
       </c>
       <c r="B83">
-        <v>14.5558555536056</v>
+        <v>17.21972341165831</v>
       </c>
       <c r="C83">
-        <v>0.1344184633129082</v>
+        <v>0.1905859568525163</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84">
-        <v>219.4449276954772</v>
+        <v>297.4839986190261</v>
       </c>
       <c r="B84">
-        <v>14.81367367318037</v>
+        <v>17.24772444756195</v>
       </c>
       <c r="C84">
-        <v>0.1456236354655849</v>
+        <v>0.1912062854171166</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85">
-        <v>235.1487152506412</v>
+        <v>293.2018158912941</v>
       </c>
       <c r="B85">
-        <v>15.33455950624736</v>
+        <v>17.12313685897809</v>
       </c>
       <c r="C85">
-        <v>0.1379456588262593</v>
+        <v>0.1884539348481855</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86">
-        <v>186.1009708967731</v>
+        <v>300.7447576883444</v>
       </c>
       <c r="B86">
-        <v>13.6418829674196</v>
+        <v>17.34199405167539</v>
       </c>
       <c r="C86">
-        <v>0.1239193996314661</v>
+        <v>0.1933021212677115</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87">
-        <v>200.399805355468</v>
+        <v>295.589833223218</v>
       </c>
       <c r="B87">
-        <v>14.15626382049544</v>
+        <v>17.19272617193731</v>
       </c>
       <c r="C87">
-        <v>0.1058241508741454</v>
+        <v>0.1899888205081495</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88">
-        <v>232.3581118043829</v>
+        <v>294.7321186822205</v>
       </c>
       <c r="B88">
-        <v>15.24329727468381</v>
+        <v>17.16776393949487</v>
       </c>
       <c r="C88">
-        <v>0.1375706053266084</v>
+        <v>0.1894375289694689</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89">
-        <v>174.5867964912632</v>
+        <v>293.6619010306105</v>
       </c>
       <c r="B89">
-        <v>13.21312970084163</v>
+        <v>17.13656619718812</v>
       </c>
       <c r="C89">
-        <v>0.1230837181651997</v>
+        <v>0.1887496521670058</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90">
-        <v>211.0902874617199</v>
+        <v>283.9405192212412</v>
       </c>
       <c r="B90">
-        <v>14.52894653654283</v>
+        <v>16.85053468650895</v>
       </c>
       <c r="C90">
-        <v>0.1376252780741543</v>
+        <v>0.1825012848144121</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91">
-        <v>214.3801283300733</v>
+        <v>299.4802638656408</v>
       </c>
       <c r="B91">
-        <v>14.64172559263673</v>
+        <v>17.30549808198657</v>
       </c>
       <c r="C91">
-        <v>0.1397379658397889</v>
+        <v>0.1924893744716002</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92">
-        <v>196.0198479832356</v>
+        <v>293.1675226786402</v>
       </c>
       <c r="B92">
-        <v>14.00070883859941</v>
+        <v>17.12213545906702</v>
       </c>
       <c r="C92">
-        <v>0.1265959358262951</v>
+        <v>0.188431893064974</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93">
-        <v>230.708982657534</v>
+        <v>294.5823170786913</v>
       </c>
       <c r="B93">
-        <v>15.18910736868806</v>
+        <v>17.16340051035025</v>
       </c>
       <c r="C93">
-        <v>0.1563990939391718</v>
+        <v>0.1893412447716836</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94">
-        <v>225.7819227465665</v>
+        <v>279.637015838407</v>
       </c>
       <c r="B94">
-        <v>15.02604148625201</v>
+        <v>16.72235078684833</v>
       </c>
       <c r="C94">
-        <v>0.1473808444286668</v>
+        <v>0.1797352305058386</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95">
-        <v>198.5372777975015</v>
+        <v>299.8747477291946</v>
       </c>
       <c r="B95">
-        <v>14.09032568103028</v>
+        <v>17.31689197659888</v>
       </c>
       <c r="C95">
-        <v>0.1279472519230002</v>
+        <v>0.1927429269132704</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96">
-        <v>199.964316613691</v>
+        <v>316.3367938562189</v>
       </c>
       <c r="B96">
-        <v>14.14087396923157</v>
+        <v>17.78585937918713</v>
       </c>
       <c r="C96">
-        <v>0.1302533335450075</v>
+        <v>0.2033238210283329</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97">
-        <v>238.6696737899771</v>
+        <v>288.7726709034101</v>
       </c>
       <c r="B97">
-        <v>15.44893762658058</v>
+        <v>16.99331253474172</v>
       </c>
       <c r="C97">
-        <v>0.1417051259397195</v>
+        <v>0.1856071250545897</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98">
-        <v>206.4837672312566</v>
+        <v>305.1870150766418</v>
       </c>
       <c r="B98">
-        <v>14.36954304183876</v>
+        <v>17.46960260213843</v>
       </c>
       <c r="C98">
-        <v>0.133763372905273</v>
+        <v>0.1961573589881495</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99">
-        <v>208.2134157467194</v>
+        <v>301.854305309369</v>
       </c>
       <c r="B99">
-        <v>14.42960206473898</v>
+        <v>17.37395479760923</v>
       </c>
       <c r="C99">
-        <v>0.1288378399921621</v>
+        <v>0.1940152772024649</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100">
-        <v>237.8233469213299</v>
+        <v>294.7610644894304</v>
       </c>
       <c r="B100">
-        <v>15.42152219858111</v>
+        <v>17.16860694667539</v>
       </c>
       <c r="C100">
-        <v>0.1547209820313283</v>
+        <v>0.189456133735776</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101">
-        <v>242.3577664997043</v>
+        <v>322.5222901203525</v>
       </c>
       <c r="B101">
-        <v>15.56784399008752</v>
+        <v>17.95890559361434</v>
       </c>
       <c r="C101">
-        <v>0.1424503124715653</v>
+        <v>0.2072995164257894</v>
       </c>
     </row>
   </sheetData>

</xml_diff>